<commit_message>
Corrected from Simon comments
</commit_message>
<xml_diff>
--- a/70 Paper/comparisonSeibel.xlsx
+++ b/70 Paper/comparisonSeibel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="13020"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -542,7 +542,7 @@
   <dimension ref="B1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +645,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="9">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="D10" s="10">
         <v>48</v>
@@ -656,7 +656,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="7">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="D11" s="8">
         <v>48</v>

</xml_diff>